<commit_message>
fix underlevel for pok skill
</commit_message>
<xml_diff>
--- a/src/universal/_data/pp/pp_gen1.xlsx
+++ b/src/universal/_data/pp/pp_gen1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6b87e023dbc3144/Desktop/pokemon/PKSM-Scripts/src/universal/clean item data/pp_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6b87e023dbc3144/Desktop/pokemon/PKSM-Scripts/src/universal/_data/pp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="11_AD4DA82427541F7ACA7EB8984011FBEC683EDF14" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{398A9C4E-38E1-4085-897E-8EAF1AA88638}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="11_AD4DA82427541F7ACA7EB8984011FBEC683EDF14" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85773478-41CF-4CCC-837D-05D2D762D831}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,34 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={16514ACB-3A4D-44F3-9DC6-C90B6480B1F4}</author>
+    <author>tc={AB29795B-D9C5-4394-A3C0-B7BA204B72AB}</author>
+  </authors>
+  <commentList>
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{16514ACB-3A4D-44F3-9DC6-C90B6480B1F4}">
+      <text>
+        <t xml:space="preserve">[Chú thích theo luồng]
+Phiên bản Excel của bạn cho phép bạn đọc chú thích theo luồng này; tuy nhiên, bất kỳ chỉnh sửa nào cho luồng cũng sẽ bị loại bỏ nếu mở tệp ở phiên bản Excel mới hơn. Tìm hiểu thêm: https://go.microsoft.com/fwlink/?linkid=870924
+Nhận xét:
+    10
+</t>
+      </text>
+    </comment>
+    <comment ref="C72" authorId="1" shapeId="0" xr:uid="{AB29795B-D9C5-4394-A3C0-B7BA204B72AB}">
+      <text>
+        <t>[Chú thích theo luồng]
+Phiên bản Excel của bạn cho phép bạn đọc chú thích theo luồng này; tuy nhiên, bất kỳ chỉnh sửa nào cho luồng cũng sẽ bị loại bỏ nếu mở tệp ở phiên bản Excel mới hơn. Tìm hiểu thêm: https://go.microsoft.com/fwlink/?linkid=870924
+Nhận xét:
+    20</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
   <si>
@@ -538,7 +566,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,6 +594,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -670,6 +704,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Trang Kiet" id="{16503DB6-1D89-4AC0-AB62-C83FCF190D9A}" userId="f6b87e023dbc3144" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -933,12 +973,24 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C23" dT="2024-08-31T17:20:31.26" personId="{16503DB6-1D89-4AC0-AB62-C83FCF190D9A}" id="{16514ACB-3A4D-44F3-9DC6-C90B6480B1F4}">
+    <text xml:space="preserve">10
+</text>
+  </threadedComment>
+  <threadedComment ref="C72" dT="2024-08-31T17:21:03.16" personId="{16503DB6-1D89-4AC0-AB62-C83FCF190D9A}" id="{AB29795B-D9C5-4394-A3C0-B7BA204B72AB}">
+    <text>20</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C166"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3106,5 +3158,6 @@
     <hyperlink ref="B36" r:id="rId330" display="https://pokemondb.net/type/normal" xr:uid="{614E22A8-F0B3-4824-8C04-35E3CD21B987}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId331"/>
 </worksheet>
 </file>
</xml_diff>